<commit_message>
Updated to address this bug: https://github.com/OpenChain-Project/Reference-Material/issues/57
</commit_message>
<xml_diff>
--- a/Adoption-Preparation/Kanban-Workflows/Community/2.0/en/Kanban-Example-1.xlsx
+++ b/Adoption-Preparation/Kanban-Workflows/Community/2.0/en/Kanban-Example-1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbain.BRUGUERAS\Documents\mbain-mmartinez\Clientes_Asuntos\FICOSA\escrits\Planif\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shane/Documents/OpenChain GitHub/Reference-Material/Adoption-Preparation/Kanban-Workflows/Community/2.0/en/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F94C60-0F43-0041-AE89-0DB24C10C859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11880" windowHeight="7980"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="19200" windowHeight="15220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -284,9 +285,6 @@
     <t>FCA</t>
   </si>
   <si>
-    <t>FOSS Compliance Artefacts</t>
-  </si>
-  <si>
     <t>generally, Review Report, Licenses, Source Code</t>
   </si>
   <si>
@@ -327,12 +325,15 @@
   </si>
   <si>
     <t>OC  FOSS Policy - PLAN</t>
+  </si>
+  <si>
+    <t>FOSS Compliance Artifact</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -395,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -433,13 +434,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -721,47 +715,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" customWidth="1"/>
-    <col min="3" max="3" width="54.7109375" customWidth="1"/>
-    <col min="4" max="4" width="41.85546875" customWidth="1"/>
-    <col min="5" max="5" width="46.85546875" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+    <col min="3" max="3" width="54.6640625" customWidth="1"/>
+    <col min="4" max="4" width="41.83203125" customWidth="1"/>
+    <col min="5" max="5" width="46.83203125" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="14"/>
       <c r="B1" s="15"/>
       <c r="C1" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D1" s="16"/>
       <c r="E1" s="15"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="18"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>83</v>
       </c>
@@ -769,7 +760,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>74</v>
       </c>
@@ -777,7 +768,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>76</v>
       </c>
@@ -785,7 +776,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>78</v>
       </c>
@@ -793,7 +784,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>80</v>
       </c>
@@ -804,37 +795,37 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>85</v>
       </c>
       <c r="C9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" t="s">
         <v>86</v>
       </c>
-      <c r="D9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" t="s">
         <v>89</v>
       </c>
-      <c r="C10" t="s">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>91</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>92</v>
       </c>
-      <c r="D11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="12" t="s">
@@ -847,7 +838,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>1</v>
       </c>
@@ -858,7 +849,7 @@
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="4"/>
       <c r="D19" t="s">
@@ -868,80 +859,80 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="4"/>
       <c r="E20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="4"/>
       <c r="D21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="4"/>
       <c r="D22" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="4"/>
       <c r="D23" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="4"/>
       <c r="E24" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="4"/>
       <c r="E25" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="4"/>
       <c r="C26" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="4"/>
       <c r="C27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="4"/>
       <c r="C28" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="4"/>
       <c r="D29" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B30" s="4"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="8">
         <v>2</v>
       </c>
@@ -952,7 +943,7 @@
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B32" s="4" t="s">
         <v>30</v>
       </c>
@@ -960,49 +951,49 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="4"/>
       <c r="D33" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="4"/>
       <c r="D34" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="4"/>
       <c r="C35" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="4"/>
       <c r="C36" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="4"/>
       <c r="C37" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="4"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" s="4"/>
       <c r="C39" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B41" s="4" t="s">
         <v>31</v>
       </c>
@@ -1010,139 +1001,139 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" s="4"/>
       <c r="C42" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B43" s="4"/>
       <c r="D43" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B44" s="4"/>
       <c r="D44" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" s="4"/>
       <c r="D45" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B46" s="4"/>
       <c r="D46" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B47" s="4"/>
       <c r="D47" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B48" s="4"/>
       <c r="D48" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B49" s="4"/>
       <c r="C49" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B50" s="4"/>
       <c r="C50" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B51" s="4"/>
       <c r="D51" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B52" s="4"/>
       <c r="D52" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B53" s="4"/>
       <c r="C53" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B54" s="4"/>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B55" s="4"/>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B56" s="4"/>
       <c r="C56" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B57" s="4"/>
       <c r="C57" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B58" s="4"/>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B59" s="4"/>
       <c r="D59" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B60" s="4"/>
       <c r="C60" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B61" s="4"/>
       <c r="C61" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B62" s="4"/>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B63" s="4"/>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B64" s="4"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B65" s="4"/>
       <c r="C65" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B66" s="4"/>
       <c r="C66" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B67" s="4" t="s">
         <v>32</v>
       </c>
@@ -1150,25 +1141,25 @@
         <v>22</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B68" s="4"/>
       <c r="C68" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B69" s="4"/>
       <c r="C69" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B70" s="4"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B71" s="4"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="8">
         <v>3</v>
       </c>
@@ -1179,7 +1170,7 @@
       <c r="D72" s="7"/>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B73" s="4" t="s">
         <v>29</v>
       </c>
@@ -1187,40 +1178,40 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B74" s="4"/>
       <c r="D74" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B75" s="4"/>
       <c r="D75" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B76" s="4"/>
       <c r="D76" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B77" s="4"/>
       <c r="C77" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B78" s="4"/>
       <c r="C78" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B79" s="4"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B80" s="4" t="s">
         <v>28</v>
       </c>
@@ -1228,36 +1219,36 @@
         <v>27</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B81" s="4"/>
       <c r="C81" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B82" s="4"/>
       <c r="C82" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B83" s="4"/>
       <c r="C83" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B84" s="4"/>
       <c r="C84" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C85" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B88" s="4" t="s">
         <v>34</v>
       </c>
@@ -1265,16 +1256,16 @@
         <v>51</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B89" s="4"/>
       <c r="C89" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B90" s="4"/>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B91" s="4" t="s">
         <v>46</v>
       </c>
@@ -1282,25 +1273,25 @@
         <v>56</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B92" s="4"/>
       <c r="C92" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B93" s="4"/>
       <c r="C93" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B94" s="4"/>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B95" s="4"/>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="8">
         <v>4</v>
       </c>
@@ -1311,28 +1302,28 @@
       <c r="D96" s="7"/>
       <c r="E96" s="7"/>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B97" s="4"/>
       <c r="C97" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C98" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C99" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C100" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="13">
         <v>5</v>
       </c>
@@ -1343,12 +1334,12 @@
       <c r="D104" s="9"/>
       <c r="E104" s="9"/>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C105" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C106" t="s">
         <v>69</v>
       </c>

</xml_diff>